<commit_message>
Committing changes from aug 23rd. JSON map is not working.
</commit_message>
<xml_diff>
--- a/app/config/tables/deployment/forms/deploy_to_beneficiary/deploy_to_beneficiary.xlsx
+++ b/app/config/tables/deployment/forms/deploy_to_beneficiary/deploy_to_beneficiary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="119">
   <si>
     <t>type</t>
   </si>
@@ -378,6 +378,9 @@
   </si>
   <si>
     <t>item_pack_name_query</t>
+  </si>
+  <si>
+    <t>number</t>
   </si>
 </sst>
 </file>
@@ -1007,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26" defaultRowHeight="23" x14ac:dyDescent="0"/>
@@ -1122,6 +1125,22 @@
       </c>
       <c r="B13" s="5" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1216,7 +1235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ODK Side is working! well for the most part
</commit_message>
<xml_diff>
--- a/app/config/tables/deployment/forms/deploy_to_beneficiary/deploy_to_beneficiary.xlsx
+++ b/app/config/tables/deployment/forms/deploy_to_beneficiary/deploy_to_beneficiary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38220" windowHeight="16780" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="120">
   <si>
     <t>type</t>
   </si>
@@ -263,9 +263,6 @@
     <t>item_pack_barcode</t>
   </si>
   <si>
-    <t>(data('scanned_item_pack_barcode') &gt; data('maxRange')) || (data('scanned_item_pack_barcode') &lt; data('minRange'))</t>
-  </si>
-  <si>
     <t>yes_no</t>
   </si>
   <si>
@@ -381,6 +378,12 @@
   </si>
   <si>
     <t>number</t>
+  </si>
+  <si>
+    <t>Please confirm or update item pack barcode</t>
+  </si>
+  <si>
+    <t>(data('item_pack_barcode') &gt; data('max_range')) || (data('item_pack_barcode') &lt; data('min_range'))</t>
   </si>
 </sst>
 </file>
@@ -1012,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26" defaultRowHeight="23" x14ac:dyDescent="0"/>
@@ -1073,7 +1076,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="4" t="s">
-        <v>2</v>
+        <v>117</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>78</v>
@@ -1084,7 +1087,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1092,7 +1095,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1100,7 +1103,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1108,7 +1111,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1116,20 +1119,20 @@
         <v>2</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>72</v>
@@ -1137,7 +1140,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>74</v>
@@ -1186,7 +1189,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1210,7 +1213,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1233,10 +1236,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0"/>
@@ -1274,7 +1277,7 @@
         <v>12</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I1" t="s">
         <v>55</v>
@@ -1377,10 +1380,10 @@
         <v>36</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1388,10 +1391,10 @@
         <v>36</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1399,10 +1402,10 @@
         <v>36</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1410,10 +1413,10 @@
         <v>36</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1426,7 +1429,7 @@
         <v>53</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1448,173 +1451,173 @@
         <v>78</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="7" t="s">
+      <c r="C18" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B19" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I19" s="16"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="C20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="I18" s="16"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="C19" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="E20" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="F20" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F19" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="I19" s="16"/>
-      <c r="J19" t="b">
+      <c r="I20" s="16"/>
+      <c r="J20" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="I20" s="16"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="7" t="s">
-        <v>84</v>
+        <v>53</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="I21" s="16"/>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="7" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="I22" s="16"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I23" s="16"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="I23" s="16"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="C24" s="4" t="s">
+      <c r="I24" s="16"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="C25" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="I24" s="16"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="26"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="28" t="s">
+      <c r="F25" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I25" s="16"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="26"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="28" t="s">
+      <c r="D26" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="29"/>
-      <c r="F25" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="G25" s="31"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="I26" s="16"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="G26" s="31"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I27" s="16"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="I27" s="22"/>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="C28" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F28" s="13" t="s">
-        <v>97</v>
       </c>
       <c r="I28" s="22"/>
     </row>
     <row r="29" spans="1:10">
       <c r="C29" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="I29" s="22"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="C30" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E29" s="5" t="s">
+      <c r="D30" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
-      <c r="I30" s="22"/>
-    </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="7" t="s">
-        <v>46</v>
-      </c>
       <c r="I31" s="22"/>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I32" s="22"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B33" s="7" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="C33" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F33" s="13" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="C34" s="4" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I34" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="C35" s="4" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F35" s="13" t="s">
-        <v>57</v>
+        <v>19</v>
+      </c>
+      <c r="I35" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1622,101 +1625,112 @@
         <v>2</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="C37" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="C38" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E38" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F37" s="13" t="s">
+      <c r="F38" s="13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="7" t="s">
+    <row r="39" spans="1:10">
+      <c r="A39" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
-      <c r="C39" s="4" t="s">
+    <row r="40" spans="1:10">
+      <c r="C40" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D40" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E40" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E39" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F39" s="13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>83</v>
+      <c r="F40" s="13" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="7" t="s">
-        <v>84</v>
+        <v>53</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
-      <c r="C43" s="4" t="s">
+    <row r="44" spans="1:10">
+      <c r="C44" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E44" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F44" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="F43" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="J43" t="b">
+      <c r="J44" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E44" s="2"/>
-      <c r="F44" s="11"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="7" t="s">
         <v>64</v>
       </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="11"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
-      <c r="C47" s="4" t="s">
+    <row r="48" spans="1:10">
+      <c r="C48" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F47" s="13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="7" t="s">
+      <c r="F48" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="7" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1858,7 +1872,7 @@
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5" t="s">
         <v>32</v>
@@ -1928,7 +1942,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
         <v>31</v>
@@ -1954,7 +1968,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B9" t="s">
         <v>31</v>
@@ -1972,7 +1986,7 @@
         <v>51</v>
       </c>
       <c r="G9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H9" s="19" t="s">
         <v>52</v>
@@ -1980,7 +1994,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B10" t="s">
         <v>31</v>
@@ -1998,7 +2012,7 @@
         <v>51</v>
       </c>
       <c r="G10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H10" s="19" t="s">
         <v>52</v>
@@ -2006,7 +2020,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B11" t="s">
         <v>31</v>
@@ -2024,7 +2038,7 @@
         <v>51</v>
       </c>
       <c r="G11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H11" s="19" t="s">
         <v>52</v>
@@ -2032,7 +2046,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B12" t="s">
         <v>31</v>
@@ -2050,7 +2064,7 @@
         <v>51</v>
       </c>
       <c r="G12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H12" s="19" t="s">
         <v>52</v>
@@ -2090,46 +2104,46 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
         <v>89</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>